<commit_message>
Add methods to export statistics
</commit_message>
<xml_diff>
--- a/intelliji/res/template.xlsx
+++ b/intelliji/res/template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="107">
   <si>
     <t xml:space="preserve">Information</t>
   </si>
@@ -352,7 +352,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -408,6 +408,13 @@
       <b val="true"/>
       <sz val="13"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -514,7 +521,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -543,7 +550,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -551,7 +562,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -559,7 +570,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -571,7 +582,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -583,11 +594,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -595,15 +606,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -696,10 +707,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,18 +784,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q72"/>
+  <dimension ref="A1:R72"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
+      <selection pane="topLeft" activeCell="P26" activeCellId="0" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4795918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.9234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,7 +862,10 @@
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="n">
+        <f aca="false">B72</f>
+        <v>0</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -866,7 +878,10 @@
       <c r="L4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="4"/>
+      <c r="M4" s="4" t="n">
+        <f aca="false">M24</f>
+        <v>0</v>
+      </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
@@ -959,1753 +974,1772 @@
       <c r="Q7" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="R7" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9" t="str">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10" t="str">
         <f aca="false">IFERROR(B8/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="10" t="str">
+      <c r="D8" s="9"/>
+      <c r="E8" s="11" t="str">
         <f aca="false">IFERROR(D8/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="10" t="str">
+      <c r="F8" s="9"/>
+      <c r="G8" s="11" t="str">
         <f aca="false">IFERROR(F8/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="L8" s="11" t="s">
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="L8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="12"/>
-      <c r="N8" s="13" t="str">
+      <c r="M8" s="13"/>
+      <c r="N8" s="14" t="str">
         <f aca="false">IFERROR(M8/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O8" s="12"/>
-      <c r="P8" s="13" t="str">
+      <c r="O8" s="13"/>
+      <c r="P8" s="14" t="str">
         <f aca="false">IFERROR(O8/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q8" s="12"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16" t="str">
+      <c r="B9" s="16"/>
+      <c r="C9" s="17" t="str">
         <f aca="false">IFERROR(B9/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="17" t="str">
+      <c r="D9" s="16"/>
+      <c r="E9" s="18" t="str">
         <f aca="false">IFERROR(D9/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="17" t="str">
+      <c r="F9" s="16"/>
+      <c r="G9" s="18" t="str">
         <f aca="false">IFERROR(F9/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="L9" s="18" t="s">
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="L9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="19"/>
-      <c r="N9" s="20" t="str">
+      <c r="M9" s="20"/>
+      <c r="N9" s="21" t="str">
         <f aca="false">IFERROR(M9/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O9" s="19"/>
-      <c r="P9" s="20" t="str">
+      <c r="O9" s="20"/>
+      <c r="P9" s="21" t="str">
         <f aca="false">IFERROR(O9/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q9" s="19"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9" t="str">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="str">
         <f aca="false">IFERROR(B10/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="10" t="str">
+      <c r="D10" s="9"/>
+      <c r="E10" s="11" t="str">
         <f aca="false">IFERROR(D10/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="10" t="str">
+      <c r="F10" s="9"/>
+      <c r="G10" s="11" t="str">
         <f aca="false">IFERROR(F10/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="L10" s="11" t="s">
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="L10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="12"/>
-      <c r="N10" s="13" t="str">
+      <c r="M10" s="13"/>
+      <c r="N10" s="14" t="str">
         <f aca="false">IFERROR(M10/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O10" s="12"/>
-      <c r="P10" s="13" t="str">
+      <c r="O10" s="13"/>
+      <c r="P10" s="14" t="str">
         <f aca="false">IFERROR(O10/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q10" s="12"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16" t="str">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17" t="str">
         <f aca="false">IFERROR(B11/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="17" t="str">
+      <c r="D11" s="16"/>
+      <c r="E11" s="18" t="str">
         <f aca="false">IFERROR(D11/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="17" t="str">
+      <c r="F11" s="16"/>
+      <c r="G11" s="18" t="str">
         <f aca="false">IFERROR(F11/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="L11" s="18" t="s">
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="L11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="M11" s="19"/>
-      <c r="N11" s="20" t="str">
+      <c r="M11" s="20"/>
+      <c r="N11" s="21" t="str">
         <f aca="false">IFERROR(M11/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O11" s="19"/>
-      <c r="P11" s="20" t="str">
+      <c r="O11" s="20"/>
+      <c r="P11" s="21" t="str">
         <f aca="false">IFERROR(O11/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q11" s="19"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9" t="str">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10" t="str">
         <f aca="false">IFERROR(B12/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="10" t="str">
+      <c r="D12" s="9"/>
+      <c r="E12" s="11" t="str">
         <f aca="false">IFERROR(D12/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="10" t="str">
+      <c r="F12" s="9"/>
+      <c r="G12" s="11" t="str">
         <f aca="false">IFERROR(F12/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="L12" s="11" t="s">
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="L12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="M12" s="12"/>
-      <c r="N12" s="13" t="str">
+      <c r="M12" s="13"/>
+      <c r="N12" s="14" t="str">
         <f aca="false">IFERROR(M12/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O12" s="12"/>
-      <c r="P12" s="13" t="str">
+      <c r="O12" s="13"/>
+      <c r="P12" s="14" t="str">
         <f aca="false">IFERROR(O12/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q12" s="12"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16" t="str">
+      <c r="B13" s="16"/>
+      <c r="C13" s="17" t="str">
         <f aca="false">IFERROR(B13/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="17" t="str">
+      <c r="D13" s="16"/>
+      <c r="E13" s="18" t="str">
         <f aca="false">IFERROR(D13/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="17" t="str">
+      <c r="F13" s="16"/>
+      <c r="G13" s="18" t="str">
         <f aca="false">IFERROR(F13/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="L13" s="18" t="s">
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="L13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="M13" s="19"/>
-      <c r="N13" s="20" t="str">
+      <c r="M13" s="20"/>
+      <c r="N13" s="21" t="str">
         <f aca="false">IFERROR(M13/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O13" s="19"/>
-      <c r="P13" s="20" t="str">
+      <c r="O13" s="20"/>
+      <c r="P13" s="21" t="str">
         <f aca="false">IFERROR(O13/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q13" s="19"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9" t="str">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="str">
         <f aca="false">IFERROR(B14/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="10" t="str">
+      <c r="D14" s="9"/>
+      <c r="E14" s="11" t="str">
         <f aca="false">IFERROR(D14/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="10" t="str">
+      <c r="F14" s="9"/>
+      <c r="G14" s="11" t="str">
         <f aca="false">IFERROR(F14/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="L14" s="11" t="s">
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="L14" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="13" t="str">
+      <c r="M14" s="13"/>
+      <c r="N14" s="14" t="str">
         <f aca="false">IFERROR(M14/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O14" s="12"/>
-      <c r="P14" s="13" t="str">
+      <c r="O14" s="13"/>
+      <c r="P14" s="14" t="str">
         <f aca="false">IFERROR(O14/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q14" s="12"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16" t="str">
+      <c r="B15" s="16"/>
+      <c r="C15" s="17" t="str">
         <f aca="false">IFERROR(B15/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="17" t="str">
+      <c r="D15" s="16"/>
+      <c r="E15" s="18" t="str">
         <f aca="false">IFERROR(D15/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="17" t="str">
+      <c r="F15" s="16"/>
+      <c r="G15" s="18" t="str">
         <f aca="false">IFERROR(F15/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="L15" s="18" t="s">
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="L15" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="M15" s="19"/>
-      <c r="N15" s="20" t="str">
+      <c r="M15" s="20"/>
+      <c r="N15" s="21" t="str">
         <f aca="false">IFERROR(M15/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O15" s="19"/>
-      <c r="P15" s="20" t="str">
+      <c r="O15" s="20"/>
+      <c r="P15" s="21" t="str">
         <f aca="false">IFERROR(O15/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q15" s="19"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9" t="str">
+      <c r="B16" s="9"/>
+      <c r="C16" s="10" t="str">
         <f aca="false">IFERROR(B16/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="10" t="str">
+      <c r="D16" s="9"/>
+      <c r="E16" s="11" t="str">
         <f aca="false">IFERROR(D16/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="10" t="str">
+      <c r="F16" s="9"/>
+      <c r="G16" s="11" t="str">
         <f aca="false">IFERROR(F16/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="L16" s="11" t="s">
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="L16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="M16" s="12"/>
-      <c r="N16" s="13" t="str">
+      <c r="M16" s="13"/>
+      <c r="N16" s="14" t="str">
         <f aca="false">IFERROR(M16/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O16" s="12"/>
-      <c r="P16" s="13" t="str">
+      <c r="O16" s="13"/>
+      <c r="P16" s="14" t="str">
         <f aca="false">IFERROR(O16/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q16" s="12"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16" t="str">
+      <c r="B17" s="16"/>
+      <c r="C17" s="17" t="str">
         <f aca="false">IFERROR(B17/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="17" t="str">
+      <c r="D17" s="16"/>
+      <c r="E17" s="18" t="str">
         <f aca="false">IFERROR(D17/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="17" t="str">
+      <c r="F17" s="16"/>
+      <c r="G17" s="18" t="str">
         <f aca="false">IFERROR(F17/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="L17" s="18" t="s">
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="L17" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="M17" s="19"/>
-      <c r="N17" s="20" t="str">
+      <c r="M17" s="20"/>
+      <c r="N17" s="21" t="str">
         <f aca="false">IFERROR(M17/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O17" s="19"/>
-      <c r="P17" s="20" t="str">
+      <c r="O17" s="20"/>
+      <c r="P17" s="21" t="str">
         <f aca="false">IFERROR(O17/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q17" s="19"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9" t="str">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10" t="str">
         <f aca="false">IFERROR(B18/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="10" t="str">
+      <c r="D18" s="9"/>
+      <c r="E18" s="11" t="str">
         <f aca="false">IFERROR(D18/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="10" t="str">
+      <c r="F18" s="9"/>
+      <c r="G18" s="11" t="str">
         <f aca="false">IFERROR(F18/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="L18" s="11" t="s">
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="L18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="M18" s="12"/>
-      <c r="N18" s="13" t="str">
+      <c r="M18" s="13"/>
+      <c r="N18" s="14" t="str">
         <f aca="false">IFERROR(M18/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O18" s="12"/>
-      <c r="P18" s="13" t="str">
+      <c r="O18" s="13"/>
+      <c r="P18" s="14" t="str">
         <f aca="false">IFERROR(O18/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q18" s="12"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16" t="str">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="str">
         <f aca="false">IFERROR(B19/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="17" t="str">
+      <c r="D19" s="16"/>
+      <c r="E19" s="18" t="str">
         <f aca="false">IFERROR(D19/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="17" t="str">
+      <c r="F19" s="16"/>
+      <c r="G19" s="18" t="str">
         <f aca="false">IFERROR(F19/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="L19" s="18" t="s">
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="L19" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="19"/>
-      <c r="N19" s="20" t="str">
+      <c r="M19" s="20"/>
+      <c r="N19" s="21" t="str">
         <f aca="false">IFERROR(M19/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O19" s="19"/>
-      <c r="P19" s="20" t="str">
+      <c r="O19" s="20"/>
+      <c r="P19" s="21" t="str">
         <f aca="false">IFERROR(O19/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q19" s="19"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9" t="str">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10" t="str">
         <f aca="false">IFERROR(B20/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="10" t="str">
+      <c r="D20" s="9"/>
+      <c r="E20" s="11" t="str">
         <f aca="false">IFERROR(D20/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="10" t="str">
+      <c r="F20" s="9"/>
+      <c r="G20" s="11" t="str">
         <f aca="false">IFERROR(F20/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="L20" s="11" t="s">
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="L20" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="M20" s="12"/>
-      <c r="N20" s="13" t="str">
+      <c r="M20" s="13"/>
+      <c r="N20" s="14" t="str">
         <f aca="false">IFERROR(M20/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O20" s="12"/>
-      <c r="P20" s="13" t="str">
+      <c r="O20" s="13"/>
+      <c r="P20" s="14" t="str">
         <f aca="false">IFERROR(O20/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q20" s="12"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16" t="str">
+      <c r="B21" s="16"/>
+      <c r="C21" s="17" t="str">
         <f aca="false">IFERROR(B21/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="17" t="str">
+      <c r="D21" s="16"/>
+      <c r="E21" s="18" t="str">
         <f aca="false">IFERROR(D21/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="17" t="str">
+      <c r="F21" s="16"/>
+      <c r="G21" s="18" t="str">
         <f aca="false">IFERROR(F21/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="L21" s="18" t="s">
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="L21" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="M21" s="19"/>
-      <c r="N21" s="20" t="str">
+      <c r="M21" s="20"/>
+      <c r="N21" s="21" t="str">
         <f aca="false">IFERROR(M21/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O21" s="19"/>
-      <c r="P21" s="20" t="str">
+      <c r="O21" s="20"/>
+      <c r="P21" s="21" t="str">
         <f aca="false">IFERROR(O21/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q21" s="19"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9" t="str">
+      <c r="B22" s="9"/>
+      <c r="C22" s="10" t="str">
         <f aca="false">IFERROR(B22/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="10" t="str">
+      <c r="D22" s="9"/>
+      <c r="E22" s="11" t="str">
         <f aca="false">IFERROR(D22/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="10" t="str">
+      <c r="F22" s="9"/>
+      <c r="G22" s="11" t="str">
         <f aca="false">IFERROR(F22/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="L22" s="11" t="s">
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="L22" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="M22" s="12"/>
-      <c r="N22" s="13" t="str">
+      <c r="M22" s="13"/>
+      <c r="N22" s="14" t="str">
         <f aca="false">IFERROR(M22/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O22" s="12"/>
-      <c r="P22" s="13" t="str">
+      <c r="O22" s="13"/>
+      <c r="P22" s="14" t="str">
         <f aca="false">IFERROR(O22/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q22" s="12"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16" t="str">
+      <c r="B23" s="16"/>
+      <c r="C23" s="17" t="str">
         <f aca="false">IFERROR(B23/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="17" t="str">
+      <c r="D23" s="16"/>
+      <c r="E23" s="18" t="str">
         <f aca="false">IFERROR(D23/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="17" t="str">
+      <c r="F23" s="16"/>
+      <c r="G23" s="18" t="str">
         <f aca="false">IFERROR(F23/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="L23" s="18" t="s">
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="L23" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="M23" s="19"/>
-      <c r="N23" s="20" t="str">
+      <c r="M23" s="20"/>
+      <c r="N23" s="21" t="str">
         <f aca="false">IFERROR(M23/$M$24*100,"")</f>
         <v/>
       </c>
-      <c r="O23" s="19"/>
-      <c r="P23" s="20" t="str">
+      <c r="O23" s="20"/>
+      <c r="P23" s="21" t="str">
         <f aca="false">IFERROR(O23/$O$24*100,"")</f>
         <v/>
       </c>
-      <c r="Q23" s="19"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9" t="str">
+      <c r="B24" s="9"/>
+      <c r="C24" s="10" t="str">
         <f aca="false">IFERROR(B24/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="10" t="str">
+      <c r="D24" s="9"/>
+      <c r="E24" s="11" t="str">
         <f aca="false">IFERROR(D24/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="10" t="str">
+      <c r="F24" s="9"/>
+      <c r="G24" s="11" t="str">
         <f aca="false">IFERROR(F24/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="L24" s="21" t="s">
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="L24" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="M24" s="21" t="n">
+      <c r="M24" s="22" t="n">
         <f aca="false">SUM(M8:M23)</f>
         <v>0</v>
       </c>
-      <c r="N24" s="21" t="n">
+      <c r="N24" s="22" t="n">
         <f aca="false">ROUND(SUM(N8:N23),0)</f>
         <v>0</v>
       </c>
-      <c r="O24" s="21" t="n">
+      <c r="O24" s="22" t="n">
         <f aca="false">SUM(O8:O23)</f>
         <v>0</v>
       </c>
-      <c r="P24" s="21" t="n">
+      <c r="P24" s="22" t="n">
         <f aca="false">ROUND(SUM(P8:KP23),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="16" t="str">
+      <c r="B25" s="16"/>
+      <c r="C25" s="17" t="str">
         <f aca="false">IFERROR(B25/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="17" t="str">
+      <c r="D25" s="16"/>
+      <c r="E25" s="18" t="str">
         <f aca="false">IFERROR(D25/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="17" t="str">
+      <c r="F25" s="16"/>
+      <c r="G25" s="18" t="str">
         <f aca="false">IFERROR(F25/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9" t="str">
+      <c r="B26" s="9"/>
+      <c r="C26" s="10" t="str">
         <f aca="false">IFERROR(B26/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="10" t="str">
+      <c r="D26" s="9"/>
+      <c r="E26" s="11" t="str">
         <f aca="false">IFERROR(D26/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="10" t="str">
+      <c r="F26" s="9"/>
+      <c r="G26" s="11" t="str">
         <f aca="false">IFERROR(F26/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="16" t="str">
+      <c r="B27" s="16"/>
+      <c r="C27" s="17" t="str">
         <f aca="false">IFERROR(B27/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="17" t="str">
+      <c r="D27" s="16"/>
+      <c r="E27" s="18" t="str">
         <f aca="false">IFERROR(D27/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="17" t="str">
+      <c r="F27" s="16"/>
+      <c r="G27" s="18" t="str">
         <f aca="false">IFERROR(F27/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9" t="str">
+      <c r="B28" s="9"/>
+      <c r="C28" s="10" t="str">
         <f aca="false">IFERROR(B28/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="10" t="str">
+      <c r="D28" s="9"/>
+      <c r="E28" s="11" t="str">
         <f aca="false">IFERROR(D28/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="10" t="str">
+      <c r="F28" s="9"/>
+      <c r="G28" s="11" t="str">
         <f aca="false">IFERROR(F28/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="16" t="str">
+      <c r="B29" s="16"/>
+      <c r="C29" s="17" t="str">
         <f aca="false">IFERROR(B29/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="17" t="str">
+      <c r="D29" s="16"/>
+      <c r="E29" s="18" t="str">
         <f aca="false">IFERROR(D29/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="17" t="str">
+      <c r="F29" s="16"/>
+      <c r="G29" s="18" t="str">
         <f aca="false">IFERROR(F29/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="9" t="str">
+      <c r="B30" s="9"/>
+      <c r="C30" s="10" t="str">
         <f aca="false">IFERROR(B30/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="10" t="str">
+      <c r="D30" s="9"/>
+      <c r="E30" s="11" t="str">
         <f aca="false">IFERROR(D30/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="10" t="str">
+      <c r="F30" s="9"/>
+      <c r="G30" s="11" t="str">
         <f aca="false">IFERROR(F30/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="16" t="str">
+      <c r="B31" s="16"/>
+      <c r="C31" s="17" t="str">
         <f aca="false">IFERROR(B31/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="17" t="str">
+      <c r="D31" s="16"/>
+      <c r="E31" s="18" t="str">
         <f aca="false">IFERROR(D31/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F31" s="15"/>
-      <c r="G31" s="17" t="str">
+      <c r="F31" s="16"/>
+      <c r="G31" s="18" t="str">
         <f aca="false">IFERROR(F31/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9" t="str">
+      <c r="B32" s="9"/>
+      <c r="C32" s="10" t="str">
         <f aca="false">IFERROR(B32/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="10" t="str">
+      <c r="D32" s="9"/>
+      <c r="E32" s="11" t="str">
         <f aca="false">IFERROR(D32/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="10" t="str">
+      <c r="F32" s="9"/>
+      <c r="G32" s="11" t="str">
         <f aca="false">IFERROR(F32/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="16" t="str">
+      <c r="B33" s="16"/>
+      <c r="C33" s="17" t="str">
         <f aca="false">IFERROR(B33/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="17" t="str">
+      <c r="D33" s="16"/>
+      <c r="E33" s="18" t="str">
         <f aca="false">IFERROR(D33/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="17" t="str">
+      <c r="F33" s="16"/>
+      <c r="G33" s="18" t="str">
         <f aca="false">IFERROR(F33/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9" t="str">
+      <c r="B34" s="9"/>
+      <c r="C34" s="10" t="str">
         <f aca="false">IFERROR(B34/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="10" t="str">
+      <c r="D34" s="9"/>
+      <c r="E34" s="11" t="str">
         <f aca="false">IFERROR(D34/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="10" t="str">
+      <c r="F34" s="9"/>
+      <c r="G34" s="11" t="str">
         <f aca="false">IFERROR(F34/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="16" t="str">
+      <c r="B35" s="16"/>
+      <c r="C35" s="17" t="str">
         <f aca="false">IFERROR(B35/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D35" s="15"/>
-      <c r="E35" s="17" t="str">
+      <c r="D35" s="16"/>
+      <c r="E35" s="18" t="str">
         <f aca="false">IFERROR(D35/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F35" s="15"/>
-      <c r="G35" s="17" t="str">
+      <c r="F35" s="16"/>
+      <c r="G35" s="18" t="str">
         <f aca="false">IFERROR(F35/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="9" t="str">
+      <c r="B36" s="9"/>
+      <c r="C36" s="10" t="str">
         <f aca="false">IFERROR(B36/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="10" t="str">
+      <c r="D36" s="9"/>
+      <c r="E36" s="11" t="str">
         <f aca="false">IFERROR(D36/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="10" t="str">
+      <c r="F36" s="9"/>
+      <c r="G36" s="11" t="str">
         <f aca="false">IFERROR(F36/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="16" t="str">
+      <c r="B37" s="16"/>
+      <c r="C37" s="17" t="str">
         <f aca="false">IFERROR(B37/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D37" s="15"/>
-      <c r="E37" s="17" t="str">
+      <c r="D37" s="16"/>
+      <c r="E37" s="18" t="str">
         <f aca="false">IFERROR(D37/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F37" s="15"/>
-      <c r="G37" s="17" t="str">
+      <c r="F37" s="16"/>
+      <c r="G37" s="18" t="str">
         <f aca="false">IFERROR(F37/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="9" t="str">
+      <c r="B38" s="9"/>
+      <c r="C38" s="10" t="str">
         <f aca="false">IFERROR(B38/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="10" t="str">
+      <c r="D38" s="9"/>
+      <c r="E38" s="11" t="str">
         <f aca="false">IFERROR(D38/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="10" t="str">
+      <c r="F38" s="9"/>
+      <c r="G38" s="11" t="str">
         <f aca="false">IFERROR(F38/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="15"/>
-      <c r="C39" s="16" t="str">
+      <c r="B39" s="16"/>
+      <c r="C39" s="17" t="str">
         <f aca="false">IFERROR(B39/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D39" s="15"/>
-      <c r="E39" s="17" t="str">
+      <c r="D39" s="16"/>
+      <c r="E39" s="18" t="str">
         <f aca="false">IFERROR(D39/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F39" s="15"/>
-      <c r="G39" s="17" t="str">
+      <c r="F39" s="16"/>
+      <c r="G39" s="18" t="str">
         <f aca="false">IFERROR(F39/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="9" t="str">
+      <c r="B40" s="9"/>
+      <c r="C40" s="10" t="str">
         <f aca="false">IFERROR(B40/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="10" t="str">
+      <c r="D40" s="9"/>
+      <c r="E40" s="11" t="str">
         <f aca="false">IFERROR(D40/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F40" s="8"/>
-      <c r="G40" s="10" t="str">
+      <c r="F40" s="9"/>
+      <c r="G40" s="11" t="str">
         <f aca="false">IFERROR(F40/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="16" t="str">
+      <c r="B41" s="16"/>
+      <c r="C41" s="17" t="str">
         <f aca="false">IFERROR(B41/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D41" s="15"/>
-      <c r="E41" s="17" t="str">
+      <c r="D41" s="16"/>
+      <c r="E41" s="18" t="str">
         <f aca="false">IFERROR(D41/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F41" s="15"/>
-      <c r="G41" s="17" t="str">
+      <c r="F41" s="16"/>
+      <c r="G41" s="18" t="str">
         <f aca="false">IFERROR(F41/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="9" t="str">
+      <c r="B42" s="9"/>
+      <c r="C42" s="10" t="str">
         <f aca="false">IFERROR(B42/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="10" t="str">
+      <c r="D42" s="9"/>
+      <c r="E42" s="11" t="str">
         <f aca="false">IFERROR(D42/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F42" s="8"/>
-      <c r="G42" s="10" t="str">
+      <c r="F42" s="9"/>
+      <c r="G42" s="11" t="str">
         <f aca="false">IFERROR(F42/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="15"/>
-      <c r="C43" s="16" t="str">
+      <c r="B43" s="16"/>
+      <c r="C43" s="17" t="str">
         <f aca="false">IFERROR(B43/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D43" s="15"/>
-      <c r="E43" s="17" t="str">
+      <c r="D43" s="16"/>
+      <c r="E43" s="18" t="str">
         <f aca="false">IFERROR(D43/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F43" s="15"/>
-      <c r="G43" s="17" t="str">
+      <c r="F43" s="16"/>
+      <c r="G43" s="18" t="str">
         <f aca="false">IFERROR(F43/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="9" t="str">
+      <c r="B44" s="9"/>
+      <c r="C44" s="10" t="str">
         <f aca="false">IFERROR(B44/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="10" t="str">
+      <c r="D44" s="9"/>
+      <c r="E44" s="11" t="str">
         <f aca="false">IFERROR(D44/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="10" t="str">
+      <c r="F44" s="9"/>
+      <c r="G44" s="11" t="str">
         <f aca="false">IFERROR(F44/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="15"/>
-      <c r="C45" s="16" t="str">
+      <c r="B45" s="16"/>
+      <c r="C45" s="17" t="str">
         <f aca="false">IFERROR(B45/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="17" t="str">
+      <c r="D45" s="16"/>
+      <c r="E45" s="18" t="str">
         <f aca="false">IFERROR(D45/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F45" s="15"/>
-      <c r="G45" s="17" t="str">
+      <c r="F45" s="16"/>
+      <c r="G45" s="18" t="str">
         <f aca="false">IFERROR(F45/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="9" t="str">
+      <c r="B46" s="9"/>
+      <c r="C46" s="10" t="str">
         <f aca="false">IFERROR(B46/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="10" t="str">
+      <c r="D46" s="9"/>
+      <c r="E46" s="11" t="str">
         <f aca="false">IFERROR(D46/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F46" s="8"/>
-      <c r="G46" s="10" t="str">
+      <c r="F46" s="9"/>
+      <c r="G46" s="11" t="str">
         <f aca="false">IFERROR(F46/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="15"/>
-      <c r="C47" s="16" t="str">
+      <c r="B47" s="16"/>
+      <c r="C47" s="17" t="str">
         <f aca="false">IFERROR(B47/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D47" s="15"/>
-      <c r="E47" s="17" t="str">
+      <c r="D47" s="16"/>
+      <c r="E47" s="18" t="str">
         <f aca="false">IFERROR(D47/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F47" s="15"/>
-      <c r="G47" s="17" t="str">
+      <c r="F47" s="16"/>
+      <c r="G47" s="18" t="str">
         <f aca="false">IFERROR(F47/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="9" t="str">
+      <c r="B48" s="9"/>
+      <c r="C48" s="10" t="str">
         <f aca="false">IFERROR(B48/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="10" t="str">
+      <c r="D48" s="9"/>
+      <c r="E48" s="11" t="str">
         <f aca="false">IFERROR(D48/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F48" s="8"/>
-      <c r="G48" s="10" t="str">
+      <c r="F48" s="9"/>
+      <c r="G48" s="11" t="str">
         <f aca="false">IFERROR(F48/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="16" t="str">
+      <c r="B49" s="16"/>
+      <c r="C49" s="17" t="str">
         <f aca="false">IFERROR(B49/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D49" s="15"/>
-      <c r="E49" s="17" t="str">
+      <c r="D49" s="16"/>
+      <c r="E49" s="18" t="str">
         <f aca="false">IFERROR(D49/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F49" s="15"/>
-      <c r="G49" s="17" t="str">
+      <c r="F49" s="16"/>
+      <c r="G49" s="18" t="str">
         <f aca="false">IFERROR(F49/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="9" t="str">
+      <c r="B50" s="9"/>
+      <c r="C50" s="10" t="str">
         <f aca="false">IFERROR(B50/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="10" t="str">
+      <c r="D50" s="9"/>
+      <c r="E50" s="11" t="str">
         <f aca="false">IFERROR(D50/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F50" s="8"/>
-      <c r="G50" s="10" t="str">
+      <c r="F50" s="9"/>
+      <c r="G50" s="11" t="str">
         <f aca="false">IFERROR(F50/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="15"/>
-      <c r="C51" s="16" t="str">
+      <c r="B51" s="16"/>
+      <c r="C51" s="17" t="str">
         <f aca="false">IFERROR(B51/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D51" s="15"/>
-      <c r="E51" s="17" t="str">
+      <c r="D51" s="16"/>
+      <c r="E51" s="18" t="str">
         <f aca="false">IFERROR(D51/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F51" s="15"/>
-      <c r="G51" s="17" t="str">
+      <c r="F51" s="16"/>
+      <c r="G51" s="18" t="str">
         <f aca="false">IFERROR(F51/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-      <c r="J51" s="15"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="9" t="str">
+      <c r="B52" s="9"/>
+      <c r="C52" s="10" t="str">
         <f aca="false">IFERROR(B52/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="10" t="str">
+      <c r="D52" s="9"/>
+      <c r="E52" s="11" t="str">
         <f aca="false">IFERROR(D52/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F52" s="8"/>
-      <c r="G52" s="10" t="str">
+      <c r="F52" s="9"/>
+      <c r="G52" s="11" t="str">
         <f aca="false">IFERROR(F52/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="15"/>
-      <c r="C53" s="16" t="str">
+      <c r="B53" s="16"/>
+      <c r="C53" s="17" t="str">
         <f aca="false">IFERROR(B53/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D53" s="15"/>
-      <c r="E53" s="17" t="str">
+      <c r="D53" s="16"/>
+      <c r="E53" s="18" t="str">
         <f aca="false">IFERROR(D53/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F53" s="15"/>
-      <c r="G53" s="17" t="str">
+      <c r="F53" s="16"/>
+      <c r="G53" s="18" t="str">
         <f aca="false">IFERROR(F53/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="9" t="str">
+      <c r="B54" s="9"/>
+      <c r="C54" s="10" t="str">
         <f aca="false">IFERROR(B54/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D54" s="8"/>
-      <c r="E54" s="10" t="str">
+      <c r="D54" s="9"/>
+      <c r="E54" s="11" t="str">
         <f aca="false">IFERROR(D54/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F54" s="8"/>
-      <c r="G54" s="10" t="str">
+      <c r="F54" s="9"/>
+      <c r="G54" s="11" t="str">
         <f aca="false">IFERROR(F54/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="14" t="s">
+      <c r="A55" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B55" s="15"/>
-      <c r="C55" s="16" t="str">
+      <c r="B55" s="16"/>
+      <c r="C55" s="17" t="str">
         <f aca="false">IFERROR(B55/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D55" s="15"/>
-      <c r="E55" s="17" t="str">
+      <c r="D55" s="16"/>
+      <c r="E55" s="18" t="str">
         <f aca="false">IFERROR(D55/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F55" s="15"/>
-      <c r="G55" s="17" t="str">
+      <c r="F55" s="16"/>
+      <c r="G55" s="18" t="str">
         <f aca="false">IFERROR(F55/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="9" t="str">
+      <c r="B56" s="9"/>
+      <c r="C56" s="10" t="str">
         <f aca="false">IFERROR(B56/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="10" t="str">
+      <c r="D56" s="9"/>
+      <c r="E56" s="11" t="str">
         <f aca="false">IFERROR(D56/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F56" s="8"/>
-      <c r="G56" s="10" t="str">
+      <c r="F56" s="9"/>
+      <c r="G56" s="11" t="str">
         <f aca="false">IFERROR(F56/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="B57" s="15"/>
-      <c r="C57" s="16" t="str">
+      <c r="B57" s="16"/>
+      <c r="C57" s="17" t="str">
         <f aca="false">IFERROR(B57/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D57" s="15"/>
-      <c r="E57" s="17" t="str">
+      <c r="D57" s="16"/>
+      <c r="E57" s="18" t="str">
         <f aca="false">IFERROR(D57/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F57" s="15"/>
-      <c r="G57" s="17" t="str">
+      <c r="F57" s="16"/>
+      <c r="G57" s="18" t="str">
         <f aca="false">IFERROR(F57/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H57" s="15"/>
-      <c r="I57" s="15"/>
-      <c r="J57" s="15"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="9" t="str">
+      <c r="B58" s="9"/>
+      <c r="C58" s="10" t="str">
         <f aca="false">IFERROR(B58/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D58" s="8"/>
-      <c r="E58" s="10" t="str">
+      <c r="D58" s="9"/>
+      <c r="E58" s="11" t="str">
         <f aca="false">IFERROR(D58/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F58" s="8"/>
-      <c r="G58" s="10" t="str">
+      <c r="F58" s="9"/>
+      <c r="G58" s="11" t="str">
         <f aca="false">IFERROR(F58/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B59" s="15"/>
-      <c r="C59" s="16" t="str">
+      <c r="B59" s="16"/>
+      <c r="C59" s="17" t="str">
         <f aca="false">IFERROR(B59/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D59" s="15"/>
-      <c r="E59" s="17" t="str">
+      <c r="D59" s="16"/>
+      <c r="E59" s="18" t="str">
         <f aca="false">IFERROR(D59/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F59" s="15"/>
-      <c r="G59" s="17" t="str">
+      <c r="F59" s="16"/>
+      <c r="G59" s="18" t="str">
         <f aca="false">IFERROR(F59/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="9" t="str">
+      <c r="B60" s="9"/>
+      <c r="C60" s="10" t="str">
         <f aca="false">IFERROR(B60/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D60" s="8"/>
-      <c r="E60" s="10" t="str">
+      <c r="D60" s="9"/>
+      <c r="E60" s="11" t="str">
         <f aca="false">IFERROR(D60/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F60" s="8"/>
-      <c r="G60" s="10" t="str">
+      <c r="F60" s="9"/>
+      <c r="G60" s="11" t="str">
         <f aca="false">IFERROR(F60/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B61" s="15"/>
-      <c r="C61" s="16" t="str">
+      <c r="B61" s="16"/>
+      <c r="C61" s="17" t="str">
         <f aca="false">IFERROR(B61/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D61" s="15"/>
-      <c r="E61" s="17" t="str">
+      <c r="D61" s="16"/>
+      <c r="E61" s="18" t="str">
         <f aca="false">IFERROR(D61/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F61" s="15"/>
-      <c r="G61" s="17" t="str">
+      <c r="F61" s="16"/>
+      <c r="G61" s="18" t="str">
         <f aca="false">IFERROR(F61/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H61" s="15"/>
-      <c r="I61" s="15"/>
-      <c r="J61" s="15"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="9" t="str">
+      <c r="B62" s="9"/>
+      <c r="C62" s="10" t="str">
         <f aca="false">IFERROR(B62/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D62" s="8"/>
-      <c r="E62" s="10" t="str">
+      <c r="D62" s="9"/>
+      <c r="E62" s="11" t="str">
         <f aca="false">IFERROR(D62/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F62" s="8"/>
-      <c r="G62" s="10" t="str">
+      <c r="F62" s="9"/>
+      <c r="G62" s="11" t="str">
         <f aca="false">IFERROR(F62/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="8"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B63" s="15"/>
-      <c r="C63" s="16" t="str">
+      <c r="B63" s="16"/>
+      <c r="C63" s="17" t="str">
         <f aca="false">IFERROR(B63/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D63" s="15"/>
-      <c r="E63" s="17" t="str">
+      <c r="D63" s="16"/>
+      <c r="E63" s="18" t="str">
         <f aca="false">IFERROR(D63/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F63" s="15"/>
-      <c r="G63" s="17" t="str">
+      <c r="F63" s="16"/>
+      <c r="G63" s="18" t="str">
         <f aca="false">IFERROR(F63/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H63" s="15"/>
-      <c r="I63" s="15"/>
-      <c r="J63" s="15"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="16"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B64" s="8"/>
-      <c r="C64" s="9" t="str">
+      <c r="B64" s="9"/>
+      <c r="C64" s="10" t="str">
         <f aca="false">IFERROR(B64/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="10" t="str">
+      <c r="D64" s="9"/>
+      <c r="E64" s="11" t="str">
         <f aca="false">IFERROR(D64/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F64" s="8"/>
-      <c r="G64" s="10" t="str">
+      <c r="F64" s="9"/>
+      <c r="G64" s="11" t="str">
         <f aca="false">IFERROR(F64/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="8"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B65" s="15"/>
-      <c r="C65" s="16" t="str">
+      <c r="B65" s="16"/>
+      <c r="C65" s="17" t="str">
         <f aca="false">IFERROR(B65/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D65" s="15"/>
-      <c r="E65" s="17" t="str">
+      <c r="D65" s="16"/>
+      <c r="E65" s="18" t="str">
         <f aca="false">IFERROR(D65/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F65" s="15"/>
-      <c r="G65" s="17" t="str">
+      <c r="F65" s="16"/>
+      <c r="G65" s="18" t="str">
         <f aca="false">IFERROR(F65/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H65" s="15"/>
-      <c r="I65" s="15"/>
-      <c r="J65" s="15"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="9" t="str">
+      <c r="B66" s="9"/>
+      <c r="C66" s="10" t="str">
         <f aca="false">IFERROR(B66/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D66" s="8"/>
-      <c r="E66" s="10" t="str">
+      <c r="D66" s="9"/>
+      <c r="E66" s="11" t="str">
         <f aca="false">IFERROR(D66/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F66" s="8"/>
-      <c r="G66" s="10" t="str">
+      <c r="F66" s="9"/>
+      <c r="G66" s="11" t="str">
         <f aca="false">IFERROR(F66/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="8"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="14" t="s">
+      <c r="A67" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B67" s="15"/>
-      <c r="C67" s="16" t="str">
+      <c r="B67" s="16"/>
+      <c r="C67" s="17" t="str">
         <f aca="false">IFERROR(B67/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D67" s="15"/>
-      <c r="E67" s="17" t="str">
+      <c r="D67" s="16"/>
+      <c r="E67" s="18" t="str">
         <f aca="false">IFERROR(D67/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F67" s="15"/>
-      <c r="G67" s="17" t="str">
+      <c r="F67" s="16"/>
+      <c r="G67" s="18" t="str">
         <f aca="false">IFERROR(F67/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
-      <c r="J67" s="15"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="9" t="str">
+      <c r="B68" s="9"/>
+      <c r="C68" s="10" t="str">
         <f aca="false">IFERROR(B68/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D68" s="8"/>
-      <c r="E68" s="10" t="str">
+      <c r="D68" s="9"/>
+      <c r="E68" s="11" t="str">
         <f aca="false">IFERROR(D68/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F68" s="8"/>
-      <c r="G68" s="10" t="str">
+      <c r="F68" s="9"/>
+      <c r="G68" s="11" t="str">
         <f aca="false">IFERROR(F68/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H68" s="8"/>
-      <c r="I68" s="8"/>
-      <c r="J68" s="8"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="14" t="s">
+      <c r="A69" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B69" s="15"/>
-      <c r="C69" s="16" t="str">
+      <c r="B69" s="16"/>
+      <c r="C69" s="17" t="str">
         <f aca="false">IFERROR(B69/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D69" s="15"/>
-      <c r="E69" s="17" t="str">
+      <c r="D69" s="16"/>
+      <c r="E69" s="18" t="str">
         <f aca="false">IFERROR(D69/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F69" s="15"/>
-      <c r="G69" s="17" t="str">
+      <c r="F69" s="16"/>
+      <c r="G69" s="18" t="str">
         <f aca="false">IFERROR(F69/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H69" s="15"/>
-      <c r="I69" s="15"/>
-      <c r="J69" s="15"/>
+      <c r="H69" s="16"/>
+      <c r="I69" s="16"/>
+      <c r="J69" s="16"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B70" s="8"/>
-      <c r="C70" s="9" t="str">
+      <c r="B70" s="9"/>
+      <c r="C70" s="10" t="str">
         <f aca="false">IFERROR(B70/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D70" s="8"/>
-      <c r="E70" s="10" t="str">
+      <c r="D70" s="9"/>
+      <c r="E70" s="11" t="str">
         <f aca="false">IFERROR(D70/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F70" s="8"/>
-      <c r="G70" s="10" t="str">
+      <c r="F70" s="9"/>
+      <c r="G70" s="11" t="str">
         <f aca="false">IFERROR(F70/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="14" t="s">
+      <c r="A71" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="B71" s="15"/>
-      <c r="C71" s="16" t="str">
+      <c r="B71" s="16"/>
+      <c r="C71" s="17" t="str">
         <f aca="false">IFERROR(B71/$B$72*100,"")</f>
         <v/>
       </c>
-      <c r="D71" s="15"/>
-      <c r="E71" s="17" t="str">
+      <c r="D71" s="16"/>
+      <c r="E71" s="18" t="str">
         <f aca="false">IFERROR(D71/$D$72*100,"")</f>
         <v/>
       </c>
-      <c r="F71" s="15"/>
-      <c r="G71" s="17" t="str">
+      <c r="F71" s="16"/>
+      <c r="G71" s="18" t="str">
         <f aca="false">IFERROR(F71/$F$72*100,"")</f>
         <v/>
       </c>
-      <c r="H71" s="15"/>
-      <c r="I71" s="15"/>
-      <c r="J71" s="15"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="22" t="s">
+      <c r="A72" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B72" s="22" t="n">
+      <c r="B72" s="23" t="n">
         <f aca="false">SUM(B8:B71)</f>
         <v>0</v>
       </c>
-      <c r="C72" s="22" t="n">
+      <c r="C72" s="23" t="n">
         <f aca="false">ROUND(SUM(C8:C71),0)</f>
         <v>0</v>
       </c>
-      <c r="D72" s="22" t="n">
+      <c r="D72" s="23" t="n">
         <f aca="false">SUM(D8:D71)</f>
         <v>0</v>
       </c>
-      <c r="E72" s="22" t="n">
+      <c r="E72" s="23" t="n">
         <f aca="false">ROUND(SUM(E8:E71),0)</f>
         <v>0</v>
       </c>
-      <c r="F72" s="22" t="n">
+      <c r="F72" s="23" t="n">
         <f aca="false">SUM(F8:F71)</f>
         <v>0</v>
       </c>
-      <c r="G72" s="22" t="n">
+      <c r="G72" s="23" t="n">
         <f aca="false">ROUND(SUM(G8:G71),0)</f>
         <v>0</v>
       </c>
-      <c r="H72" s="23"/>
-      <c r="I72" s="23"/>
-      <c r="J72" s="23"/>
+      <c r="H72" s="24"/>
+      <c r="I72" s="24"/>
+      <c r="J72" s="24"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>